<commit_message>
add import of cmdr
</commit_message>
<xml_diff>
--- a/project/excel/linkml_map_example.xlsx
+++ b/project/excel/linkml_map_example.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,6 +506,11 @@
       <c r="L1" t="inlineStr">
         <is>
           <t>id</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>name</t>
         </is>
       </c>
     </row>

</xml_diff>